<commit_message>
#9 - api 설계 수정
hashtag 의 URL 부분 수정
</commit_message>
<xml_diff>
--- a/document/게시판api설계.xlsx
+++ b/document/게시판api설계.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\=== kh정보교육원 ===\수업\github\project-board\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3849DB-72FE-4FA5-9D76-9A7ED4A1A4C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC5548A-E276-4804-B83F-DDC80C12FA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="7380" windowWidth="24240" windowHeight="13740" xr2:uid="{150BB030-F946-48D3-B981-83732A1A8391}"/>
+    <workbookView xWindow="-23805" yWindow="8550" windowWidth="18240" windowHeight="11700" xr2:uid="{150BB030-F946-48D3-B981-83732A1A8391}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -121,10 +121,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/articles/hashtag</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>게시판 해시태그 검색 전용 페이지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -286,6 +282,10 @@
   </si>
   <si>
     <t>필터: 본문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/articles/serach/hashtag</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -442,60 +442,57 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -814,7 +811,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:D22"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -826,346 +823,346 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="12" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="4" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7" t="s">
+      <c r="D14" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="8" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="16" t="s">
+      <c r="C15" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="16" t="s">
+      <c r="E15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="17" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="B16" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="16" t="s">
+      <c r="C16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="16" t="s">
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
+      <c r="B18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="16" t="s">
+      <c r="E18" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
+      <c r="B21" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="15"/>
+      <c r="B22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="15"/>
+      <c r="B23" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
+      <c r="B24" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E24" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="15"/>
+      <c r="B25" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="16"/>
+      <c r="B26" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="13"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
-      <c r="B25" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="12" t="s">
+      <c r="D26" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E26" s="10" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
-      <c r="B26" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>